<commit_message>
sensing depth not working
</commit_message>
<xml_diff>
--- a/data/output/PC/soil_moisture/PC_soil_moisture.xlsx
+++ b/data/output/PC/soil_moisture/PC_soil_moisture.xlsx
@@ -517,7 +517,7 @@
         <v>0.4768961515609137</v>
       </c>
       <c r="I2" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J2" t="n">
         <v>235.5866988710914</v>
@@ -552,7 +552,7 @@
         <v>0.4907090233955974</v>
       </c>
       <c r="I3" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J3" t="n">
         <v>241.1100588728776</v>
@@ -587,7 +587,7 @@
         <v>0.4356852260653008</v>
       </c>
       <c r="I4" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J4" t="n">
         <v>221.2401482386922</v>
@@ -622,7 +622,7 @@
         <v>0.4294243174066552</v>
       </c>
       <c r="I5" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J5" t="n">
         <v>215.0565715170844</v>
@@ -657,7 +657,7 @@
         <v>0.4105070183952378</v>
       </c>
       <c r="I6" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J6" t="n">
         <v>206.2598606437968</v>
@@ -692,7 +692,7 @@
         <v>0.4325882074700618</v>
       </c>
       <c r="I7" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J7" t="n">
         <v>212.138457547282</v>
@@ -727,7 +727,7 @@
         <v>0.4078742690939023</v>
       </c>
       <c r="I8" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J8" t="n">
         <v>204.093976021311</v>
@@ -762,7 +762,7 @@
         <v>0.4023122986670622</v>
       </c>
       <c r="I9" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J9" t="n">
         <v>200.4154474160272</v>
@@ -797,7 +797,7 @@
         <v>0.376035111343873</v>
       </c>
       <c r="I10" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J10" t="n">
         <v>189.7594153972337</v>
@@ -832,7 +832,7 @@
         <v>0.3777768181144189</v>
       </c>
       <c r="I11" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J11" t="n">
         <v>187.8682004633052</v>
@@ -867,7 +867,7 @@
         <v>0.3329170171784661</v>
       </c>
       <c r="I12" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J12" t="n">
         <v>170.6954212171697</v>
@@ -902,7 +902,7 @@
         <v>0.3120140651479551</v>
       </c>
       <c r="I13" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J13" t="n">
         <v>159.1198267708231</v>
@@ -937,7 +937,7 @@
         <v>0.2902929820390653</v>
       </c>
       <c r="I14" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J14" t="n">
         <v>148.0353084622459</v>
@@ -972,7 +972,7 @@
         <v>0.2802601456097492</v>
       </c>
       <c r="I15" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J15" t="n">
         <v>141.4438071086929</v>
@@ -1007,7 +1007,7 @@
         <v>0.2778206258124313</v>
       </c>
       <c r="I16" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J16" t="n">
         <v>138.6594031359971</v>
@@ -1042,7 +1042,7 @@
         <v>0.263864912930071</v>
       </c>
       <c r="I17" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J17" t="n">
         <v>132.6670959223383</v>
@@ -1077,7 +1077,7 @@
         <v>0.2492252498794999</v>
       </c>
       <c r="I18" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J18" t="n">
         <v>125.8549257307175</v>
@@ -1112,7 +1112,7 @@
         <v>0.2413439865064645</v>
       </c>
       <c r="I19" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J19" t="n">
         <v>121.2458294438275</v>
@@ -1147,7 +1147,7 @@
         <v>0.2451939872486993</v>
       </c>
       <c r="I20" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J20" t="n">
         <v>121.3739275383585</v>
@@ -1182,7 +1182,7 @@
         <v>0.2349415803644948</v>
       </c>
       <c r="I21" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J21" t="n">
         <v>117.4724881892059</v>
@@ -1217,7 +1217,7 @@
         <v>0.3169665383736176</v>
       </c>
       <c r="I22" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J22" t="n">
         <v>146.539322195179</v>
@@ -1252,7 +1252,7 @@
         <v>0.3781259304022481</v>
       </c>
       <c r="I23" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J23" t="n">
         <v>175.225160880978</v>
@@ -1287,7 +1287,7 @@
         <v>0.3531553111386488</v>
       </c>
       <c r="I24" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J24" t="n">
         <v>173.417870629293</v>
@@ -1322,7 +1322,7 @@
         <v>0.3197228536001017</v>
       </c>
       <c r="I25" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J25" t="n">
         <v>161.8648710599797</v>
@@ -1357,7 +1357,7 @@
         <v>0.3036755765496637</v>
       </c>
       <c r="I26" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J26" t="n">
         <v>153.5246897182572</v>
@@ -1392,7 +1392,7 @@
         <v>0.2929974331720085</v>
       </c>
       <c r="I27" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J27" t="n">
         <v>147.4064986521406</v>
@@ -1427,7 +1427,7 @@
         <v>0.3870498820743378</v>
       </c>
       <c r="I28" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J28" t="n">
         <v>180.0733356757863</v>
@@ -1462,7 +1462,7 @@
         <v>0.3918101098068956</v>
       </c>
       <c r="I29" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J29" t="n">
         <v>188.84703487601</v>
@@ -1497,7 +1497,7 @@
         <v>0.344449805185451</v>
       </c>
       <c r="I30" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J30" t="n">
         <v>174.5245454428329</v>
@@ -1532,7 +1532,7 @@
         <v>0.3474612933649757</v>
       </c>
       <c r="I31" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J31" t="n">
         <v>172.8644136539463</v>
@@ -1567,7 +1567,7 @@
         <v>0.327834476144631</v>
       </c>
       <c r="I32" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J32" t="n">
         <v>164.9256109844224</v>
@@ -1602,7 +1602,7 @@
         <v>0.3087924015987075</v>
       </c>
       <c r="I33" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J33" t="n">
         <v>156.0898431463894</v>
@@ -1637,7 +1637,7 @@
         <v>0.28079239251543</v>
       </c>
       <c r="I34" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J34" t="n">
         <v>143.6213080526459</v>
@@ -1672,7 +1672,7 @@
         <v>0.2731209003803149</v>
       </c>
       <c r="I35" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J35" t="n">
         <v>137.7157280872388</v>
@@ -1707,7 +1707,7 @@
         <v>0.2658531243709848</v>
       </c>
       <c r="I36" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J36" t="n">
         <v>133.2950826935725</v>
@@ -1742,7 +1742,7 @@
         <v>0.2585666345583624</v>
       </c>
       <c r="I37" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J37" t="n">
         <v>129.3924924134965</v>
@@ -1777,7 +1777,7 @@
         <v>0.2600397844859729</v>
       </c>
       <c r="I38" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J38" t="n">
         <v>128.8808653673879</v>
@@ -1812,7 +1812,7 @@
         <v>0.2544595542212646</v>
       </c>
       <c r="I39" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J39" t="n">
         <v>126.5764731554106</v>
@@ -1847,7 +1847,7 @@
         <v>0.2499336485751482</v>
       </c>
       <c r="I40" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J40" t="n">
         <v>124.3712936077679</v>
@@ -1882,7 +1882,7 @@
         <v>0.2345045001740313</v>
       </c>
       <c r="I41" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J41" t="n">
         <v>118.1644355701344</v>
@@ -1917,7 +1917,7 @@
         <v>0.2364121160680182</v>
       </c>
       <c r="I42" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J42" t="n">
         <v>117.3951554960653</v>
@@ -1952,7 +1952,7 @@
         <v>0.2307081262322634</v>
       </c>
       <c r="I43" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J43" t="n">
         <v>114.9277601367352</v>
@@ -1987,7 +1987,7 @@
         <v>0.3927675762381846</v>
       </c>
       <c r="I44" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J44" t="n">
         <v>173.51317225249</v>
@@ -2022,7 +2022,7 @@
         <v>0.41340858704039</v>
       </c>
       <c r="I45" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J45" t="n">
         <v>194.0194680807457</v>
@@ -2057,7 +2057,7 @@
         <v>0.4328056796145132</v>
       </c>
       <c r="I46" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J46" t="n">
         <v>207.5544993036212</v>
@@ -2092,7 +2092,7 @@
         <v>0.4293560179920805</v>
       </c>
       <c r="I47" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J47" t="n">
         <v>210.2462430540921</v>
@@ -2127,7 +2127,7 @@
         <v>0.3986609565188758</v>
       </c>
       <c r="I48" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J48" t="n">
         <v>200.2080931754933</v>
@@ -2162,7 +2162,7 @@
         <v>0.379327386564998</v>
       </c>
       <c r="I49" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J49" t="n">
         <v>191.079888486066</v>
@@ -2197,7 +2197,7 @@
         <v>0.3914169891562055</v>
       </c>
       <c r="I50" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J50" t="n">
         <v>193.1616315393534</v>
@@ -2232,7 +2232,7 @@
         <v>0.3953603486928283</v>
       </c>
       <c r="I51" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J51" t="n">
         <v>194.7273009663018</v>
@@ -2267,7 +2267,7 @@
         <v>0.4163367303888826</v>
       </c>
       <c r="I52" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J52" t="n">
         <v>202.7558402163629</v>
@@ -2302,7 +2302,7 @@
         <v>0.5513435833091318</v>
       </c>
       <c r="I53" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J53" t="n">
         <v>253.9083578704211</v>
@@ -2337,7 +2337,7 @@
         <v>0.4620739720653525</v>
       </c>
       <c r="I54" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J54" t="n">
         <v>232.9693493020123</v>
@@ -2372,7 +2372,7 @@
         <v>0.4311930633969822</v>
       </c>
       <c r="I55" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J55" t="n">
         <v>218.7163331238376</v>
@@ -2407,7 +2407,7 @@
         <v>0.3907199248605503</v>
       </c>
       <c r="I56" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J56" t="n">
         <v>200.326348520764</v>
@@ -2442,7 +2442,7 @@
         <v>0.4031163811998669</v>
       </c>
       <c r="I57" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J57" t="n">
         <v>200.2328101173035</v>
@@ -2477,7 +2477,7 @@
         <v>0.3717213108698151</v>
       </c>
       <c r="I58" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J58" t="n">
         <v>188.0748970376515</v>
@@ -2512,7 +2512,7 @@
         <v>0.3817218058629429</v>
       </c>
       <c r="I59" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J59" t="n">
         <v>188.9179960500872</v>
@@ -2547,7 +2547,7 @@
         <v>0.3419814941718938</v>
       </c>
       <c r="I60" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J60" t="n">
         <v>174.1835435307954</v>
@@ -2582,7 +2582,7 @@
         <v>0.3417882519943188</v>
       </c>
       <c r="I61" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J61" t="n">
         <v>170.7976898614041</v>
@@ -2617,7 +2617,7 @@
         <v>0.3265550472567733</v>
       </c>
       <c r="I62" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J62" t="n">
         <v>163.9985316961058</v>
@@ -2652,7 +2652,7 @@
         <v>0.3443323840693779</v>
       </c>
       <c r="I63" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J63" t="n">
         <v>168.7972682488364</v>
@@ -2687,7 +2687,7 @@
         <v>0.3153774159504824</v>
       </c>
       <c r="I64" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J64" t="n">
         <v>159.0453006317724</v>
@@ -2722,7 +2722,7 @@
         <v>0.3178308460086563</v>
       </c>
       <c r="I65" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J65" t="n">
         <v>157.8877274143219</v>
@@ -2757,7 +2757,7 @@
         <v>0.3393529338140498</v>
       </c>
       <c r="I66" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J66" t="n">
         <v>165.1926850567532</v>
@@ -2792,7 +2792,7 @@
         <v>0.3153209456249411</v>
       </c>
       <c r="I67" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J67" t="n">
         <v>157.9624078180535</v>
@@ -2827,7 +2827,7 @@
         <v>0.3195162375719491</v>
       </c>
       <c r="I68" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J68" t="n">
         <v>158.107921021308</v>
@@ -2862,7 +2862,7 @@
         <v>0.3205913798259547</v>
       </c>
       <c r="I69" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J69" t="n">
         <v>158.3318955760186</v>
@@ -2897,7 +2897,7 @@
         <v>0.3032718168845871</v>
       </c>
       <c r="I70" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J70" t="n">
         <v>152.0315007413299</v>
@@ -2932,7 +2932,7 @@
         <v>0.2960539002480533</v>
       </c>
       <c r="I71" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J71" t="n">
         <v>147.9949248940854</v>
@@ -2967,7 +2967,7 @@
         <v>0.2982900138096482</v>
       </c>
       <c r="I72" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J72" t="n">
         <v>147.7090411859489</v>
@@ -3002,7 +3002,7 @@
         <v>0.273734636036658</v>
       </c>
       <c r="I73" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J73" t="n">
         <v>138.5167530459403</v>
@@ -3037,7 +3037,7 @@
         <v>0.2576793978367655</v>
       </c>
       <c r="I74" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J74" t="n">
         <v>130.5718610570728</v>
@@ -3072,7 +3072,7 @@
         <v>0.2615235486787043</v>
       </c>
       <c r="I75" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J75" t="n">
         <v>129.9036651819162</v>
@@ -3107,7 +3107,7 @@
         <v>0.25170703252118</v>
       </c>
       <c r="I76" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J76" t="n">
         <v>125.868801237206</v>
@@ -3142,7 +3142,7 @@
         <v>0.3082866030205854</v>
       </c>
       <c r="I77" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J77" t="n">
         <v>145.5697307036373</v>
@@ -3177,7 +3177,7 @@
         <v>0.2756542005977451</v>
       </c>
       <c r="I78" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J78" t="n">
         <v>137.9012849661177</v>
@@ -3212,7 +3212,7 @@
         <v>0.2687217922260148</v>
       </c>
       <c r="I79" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J79" t="n">
         <v>134.2769031344332</v>
@@ -3247,7 +3247,7 @@
         <v>0.3532875621886893</v>
       </c>
       <c r="I80" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J80" t="n">
         <v>164.197796899085</v>
@@ -3282,7 +3282,7 @@
         <v>0.5111507141046006</v>
       </c>
       <c r="I81" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J81" t="n">
         <v>228.3835216048609</v>
@@ -3317,7 +3317,7 @@
         <v>0.3912947987509279</v>
       </c>
       <c r="I82" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J82" t="n">
         <v>199.856948894974</v>
@@ -3352,7 +3352,7 @@
         <v>0.3894013937522755</v>
       </c>
       <c r="I83" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J83" t="n">
         <v>195.0203817803171</v>
@@ -3387,7 +3387,7 @@
         <v>0.4807496083973564</v>
       </c>
       <c r="I84" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J84" t="n">
         <v>226.7056331004698</v>
@@ -3422,7 +3422,7 @@
         <v>0.5007835610315862</v>
       </c>
       <c r="I85" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J85" t="n">
         <v>240.840091753564</v>
@@ -3457,7 +3457,7 @@
         <v>0.4210562326160445</v>
       </c>
       <c r="I86" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J86" t="n">
         <v>215.858792605975</v>
@@ -3492,7 +3492,7 @@
         <v>0.3997113484160246</v>
       </c>
       <c r="I87" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J87" t="n">
         <v>203.0961603493924</v>
@@ -3527,7 +3527,7 @@
         <v>0.4243536677290205</v>
       </c>
       <c r="I88" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J88" t="n">
         <v>208.5322026835503</v>
@@ -3562,7 +3562,7 @@
         <v>0.4185577833188718</v>
       </c>
       <c r="I89" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J89" t="n">
         <v>207.1096913695193</v>
@@ -3597,7 +3597,7 @@
         <v>0.4082899977329208</v>
       </c>
       <c r="I90" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J90" t="n">
         <v>203.143185038371</v>
@@ -3632,7 +3632,7 @@
         <v>0.3595221374535424</v>
       </c>
       <c r="I91" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J91" t="n">
         <v>184.4158407833725</v>
@@ -3667,7 +3667,7 @@
         <v>0.389826784485038</v>
       </c>
       <c r="I92" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J92" t="n">
         <v>191.1784314814672</v>

</xml_diff>